<commit_message>
Minor wording improvements in the template
</commit_message>
<xml_diff>
--- a/input/template.xlsx
+++ b/input/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chat/Seafile/2020 HS - HCI/Project/1 Instruction/Peer assessment/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chat/Seafile/2020 HS - HCI/Project/1 Instruction/Peer assessment/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440536CD-7633-4B42-85C6-FF6897710F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEEB4AE-383B-8C43-B147-FFCD2BE8C530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1320" windowWidth="20560" windowHeight="14500" xr2:uid="{50EDE1AE-5C62-B246-8B6C-A7BCEBA9A8A5}"/>
+    <workbookView xWindow="6100" yWindow="2580" windowWidth="20560" windowHeight="14500" xr2:uid="{50EDE1AE-5C62-B246-8B6C-A7BCEBA9A8A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>My name (x)</t>
   </si>
   <si>
-    <t>Step 1: In the table below, add "x" (without quotes) in column A, in the row with your name.</t>
-  </si>
-  <si>
     <t>Team</t>
   </si>
   <si>
@@ -61,6 +58,48 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Step 3: Rate the contribution of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>all</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> other team members.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">     1: Made only a small contribution or contributed in a poor standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     2: …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     3: Made an average contribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     4: …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     5: Contributed to the most challenging aspects in a high standard</t>
+  </si>
+  <si>
+    <t>Step 1: In the table below, on the row with your name, add "x" (without quotes) in column "My name (x)".</t>
   </si>
   <si>
     <r>
@@ -85,50 +124,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> contribution to the project on the range 1–5 according to the following guide:</t>
+      <t xml:space="preserve"> contribution in the column "Rating"to the project on the range 1–5 according to the following guide:</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Step 3: Rate the contribution of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>all</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> other team members.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">     1: Made only a small contribution or contributed in a poor standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     2: …</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     3: Made an average contribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     4: …</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     5: Contributed to the most challenging aspects in a high standard</t>
-  </si>
-  <si>
-    <t>Step 4: If you have any comments about any person's contribution, write in the comments column</t>
+    <t>Step 4: If you have any comments about any person's contribution, write in the "Comments" column</t>
   </si>
 </sst>
 </file>
@@ -213,6 +213,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFE699"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -524,7 +529,7 @@
   <dimension ref="A2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,42 +542,42 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -594,62 +599,62 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="4"/>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="4"/>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>